<commit_message>
updates to the data
</commit_message>
<xml_diff>
--- a/summary_of_the_results.xlsx
+++ b/summary_of_the_results.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrico.vigano/libcsp_workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62314A79-EAC4-2E40-8C2F-C26F285B4850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE446A6-6E84-0F4E-800D-2DC1F4AF2384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19080" windowHeight="21600" activeTab="1" xr2:uid="{87830DE4-77D0-D242-BBAB-3679D6DFCD25}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{87830DE4-77D0-D242-BBAB-3679D6DFCD25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sum Up" sheetId="1" r:id="rId1"/>
     <sheet name="Final Mutants Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Final Mutants Table'!$A$1:$W$59</definedName>
     <definedName name="final_mutants_table" localSheetId="1">'Final Mutants Table'!$A$1:$O$59</definedName>
     <definedName name="final_mutants_table_1" localSheetId="1">'Final Mutants Table'!$P$1:$Q$59</definedName>
     <definedName name="final_mutants_table_2" localSheetId="1">'Final Mutants Table'!$R$1:$S$59</definedName>
@@ -50,7 +51,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{B38DB730-E868-1B4D-83EE-CF38E8FAD7C3}" name="final_mutants_table" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_01/final_mutants_table.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_01/final_mutants_table.csv" thousands="'" comma="1">
       <textFields count="14">
         <textField/>
         <textField/>
@@ -70,7 +71,7 @@
     </textPr>
   </connection>
   <connection id="2" xr16:uid="{1E41F220-F84C-BA4C-81D6-CA8542472B4D}" name="final_mutants_table1" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_02/final_mutants_table.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_02/final_mutants_table.csv" thousands="'" comma="1">
       <textFields count="14">
         <textField/>
         <textField/>
@@ -90,7 +91,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{FF0B2694-ED74-F04C-A46E-3B218EF8D2DB}" name="final_mutants_table2" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_03/final_mutants_table.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_03/final_mutants_table.csv" thousands="'" comma="1">
       <textFields count="14">
         <textField/>
         <textField/>
@@ -110,7 +111,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{1F14FE8A-84A6-9C48-8F19-7E711EED9955}" name="final_mutants_table3" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_04/final_mutants_table.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_04/final_mutants_table.csv" thousands="'" comma="1">
       <textFields count="14">
         <textField/>
         <textField/>
@@ -130,7 +131,7 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{47E1CE52-0123-2149-BE63-8D17DFE4A308}" name="final_mutants_table4" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_05/final_mutants_table.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_05/final_mutants_table.csv" thousands="'" comma="1">
       <textFields count="14">
         <textField/>
         <textField/>
@@ -150,7 +151,7 @@
     </textPr>
   </connection>
   <connection id="6" xr16:uid="{447784CD-1FEA-1D42-8DBD-99EABDAB9C3B}" name="mutation_sum_up" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_01/mutation_sum_up.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_01/mutation_sum_up.csv" thousands="'" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -159,7 +160,7 @@
     </textPr>
   </connection>
   <connection id="7" xr16:uid="{2E695EAC-8EBC-B94B-947B-DC4FB787161E}" name="mutation_sum_up1" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_02/mutation_sum_up.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_02/mutation_sum_up.csv" thousands="'" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -168,7 +169,7 @@
     </textPr>
   </connection>
   <connection id="8" xr16:uid="{DB62747F-77A5-1646-A585-205300B79486}" name="mutation_sum_up2" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_03/mutation_sum_up.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_03/mutation_sum_up.csv" thousands="'" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -177,7 +178,7 @@
     </textPr>
   </connection>
   <connection id="9" xr16:uid="{D6846EE8-81C8-C947-9102-C0A666C0C70A}" name="mutation_sum_up3" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_04/mutation_sum_up.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_04/mutation_sum_up.csv" thousands="'" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -186,7 +187,7 @@
     </textPr>
   </connection>
   <connection id="10" xr16:uid="{4D0D15A4-747B-8B42-9AD3-1C1EDB6CAC46}" name="mutation_sum_up4" type="6" refreshedVersion="7" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_05/mutation_sum_up.csv" thousands="'" comma="1">
+    <textPr sourceFile="/Users/enrico.vigano/libcsp_workspace/damat-pipeline/results_test_05/mutation_sum_up.csv" thousands="'" comma="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -198,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="64">
   <si>
     <t>all_fault_models</t>
   </si>
@@ -373,6 +374,24 @@
   <si>
     <t>conn-&gt;idin.flags</t>
   </si>
+  <si>
+    <t xml:space="preserve"> conn-&gt;idout.pri</t>
+  </si>
+  <si>
+    <t>conn-&gt;idout.src</t>
+  </si>
+  <si>
+    <t>conn-&gt;idout.dst</t>
+  </si>
+  <si>
+    <t>conn-&gt;idout.dport</t>
+  </si>
+  <si>
+    <t>conn-&gt;idout.sport</t>
+  </si>
+  <si>
+    <t>conn-&gt;idout.flags</t>
+  </si>
 </sst>
 </file>
 
@@ -457,29 +476,19 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1406,7 +1415,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table" connectionId="1" xr16:uid="{C119F7E3-450F-C545-9269-FF16116AB807}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_3" connectionId="4" xr16:uid="{6DA3802D-04E6-5540-AF52-8F92362B5EEC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1426,19 +1435,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_4" connectionId="5" xr16:uid="{5D42AE49-F949-0C4A-AA9D-FC892923890F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_2" connectionId="3" xr16:uid="{E10B54AE-A433-8A44-94AF-B7174EE183B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_3" connectionId="4" xr16:uid="{6DA3802D-04E6-5540-AF52-8F92362B5EEC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_1" connectionId="2" xr16:uid="{125BD8C0-F502-3B48-94F2-0CD055221A3A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_2" connectionId="3" xr16:uid="{E10B54AE-A433-8A44-94AF-B7174EE183B4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table" connectionId="1" xr16:uid="{C119F7E3-450F-C545-9269-FF16116AB807}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_1" connectionId="2" xr16:uid="{125BD8C0-F502-3B48-94F2-0CD055221A3A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="final_mutants_table_4" connectionId="5" xr16:uid="{5D42AE49-F949-0C4A-AA9D-FC892923890F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1740,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF60103E-8BD0-B64D-9FDC-031384490C5F}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,20 +1761,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1776,18 +1785,18 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1798,18 +1807,18 @@
       <c r="B5" s="1">
         <v>44</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1820,25 +1829,25 @@
       <c r="B7" s="1">
         <v>22</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1849,18 +1858,18 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1871,18 +1880,18 @@
       <c r="B13" s="1">
         <v>44</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1893,25 +1902,25 @@
       <c r="B15" s="1">
         <v>27</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.61399999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1922,18 +1931,18 @@
       <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1944,18 +1953,18 @@
       <c r="B21" s="1">
         <v>44</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1966,25 +1975,25 @@
       <c r="B23" s="1">
         <v>32</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>0.72699999999999998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1995,18 +2004,18 @@
       <c r="B27" s="1">
         <v>2</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2017,18 +2026,18 @@
       <c r="B29" s="1">
         <v>44</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2039,25 +2048,25 @@
       <c r="B31" s="1">
         <v>36</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>0.81799999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B34" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2068,18 +2077,18 @@
       <c r="B35" s="1">
         <v>2</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -2090,18 +2099,18 @@
       <c r="B37" s="1">
         <v>44</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <v>0.75900000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2112,7 +2121,7 @@
       <c r="B39" s="1">
         <v>42</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="4">
         <v>0.95499999999999996</v>
       </c>
     </row>
@@ -2133,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D9D609-1E59-F148-BC00-A391F2F58DC2}">
   <dimension ref="A1:W59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2163,74 +2172,74 @@
     <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -4280,7 +4289,7 @@
       <c r="S30" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="T30" s="7" t="s">
+      <c r="T30" s="6" t="s">
         <v>29</v>
       </c>
       <c r="U30" s="1" t="s">
@@ -4331,7 +4340,7 @@
         <v>1</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>29</v>
@@ -4402,7 +4411,7 @@
         <v>28</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>29</v>
@@ -4473,7 +4482,7 @@
         <v>28</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>29</v>
@@ -4544,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>29</v>
@@ -4615,7 +4624,7 @@
         <v>28</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>29</v>
@@ -4686,7 +4695,7 @@
         <v>28</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>29</v>
@@ -4757,7 +4766,7 @@
         <v>1</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>34</v>
@@ -4828,7 +4837,7 @@
         <v>28</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>34</v>
@@ -4899,7 +4908,7 @@
         <v>28</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>29</v>
@@ -4970,7 +4979,7 @@
         <v>1</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>34</v>
@@ -5041,7 +5050,7 @@
         <v>28</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>34</v>
@@ -5112,7 +5121,7 @@
         <v>28</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>34</v>
@@ -5183,7 +5192,7 @@
         <v>28</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>34</v>
@@ -5254,7 +5263,7 @@
         <v>28</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>34</v>
@@ -5325,7 +5334,7 @@
         <v>28</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>34</v>
@@ -5396,7 +5405,7 @@
         <v>0</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>34</v>
@@ -5467,7 +5476,7 @@
         <v>28</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>34</v>
@@ -5538,7 +5547,7 @@
         <v>28</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>34</v>
@@ -5609,7 +5618,7 @@
         <v>28</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>34</v>
@@ -5680,7 +5689,7 @@
         <v>28</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N50" s="1" t="s">
         <v>34</v>
@@ -5751,7 +5760,7 @@
         <v>28</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="N51" s="1" t="s">
         <v>34</v>
@@ -5822,7 +5831,7 @@
         <v>1</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N52" s="1" t="s">
         <v>29</v>
@@ -5893,7 +5902,7 @@
         <v>1</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>29</v>
@@ -5964,7 +5973,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>29</v>
@@ -6035,7 +6044,7 @@
         <v>1</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>34</v>
@@ -6106,7 +6115,7 @@
         <v>1</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N56" s="1" t="s">
         <v>29</v>
@@ -6177,7 +6186,7 @@
         <v>1</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N57" s="1" t="s">
         <v>29</v>
@@ -6248,7 +6257,7 @@
         <v>1</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N58" s="1" t="s">
         <v>29</v>
@@ -6319,7 +6328,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="N59" s="1" t="s">
         <v>29</v>
@@ -6355,10 +6364,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="N2:W59">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="LIVE">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="LIVE">
       <formula>NOT(ISERROR(SEARCH("LIVE",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="KILLED">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="KILLED">
       <formula>NOT(ISERROR(SEARCH("KILLED",N2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>